<commit_message>
Finishing of the entire officer tool.
Additions are to come
</commit_message>
<xml_diff>
--- a/Misc/Crews.xlsx
+++ b/Misc/Crews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Applications\GithubRepositories\DiscordBot\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952895A1-02CD-4351-B177-8EDEC672229C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03705D13-69AC-46BB-A8B4-A9013C7A6B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FBE1628F-8245-4231-B5D1-5265D21CCCC4}"/>
+    <workbookView xWindow="2430" yWindow="1245" windowWidth="24825" windowHeight="14310" xr2:uid="{FBE1628F-8245-4231-B5D1-5265D21CCCC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
   <si>
     <t>Description</t>
   </si>
@@ -219,13 +219,64 @@
     <t>Stella Max Loot</t>
   </si>
   <si>
-    <t>Hostiles</t>
-  </si>
-  <si>
     <t>"Stonn","Two of Eleven","Four of Eleven"</t>
   </si>
   <si>
     <t>Stella crew for added cargo, you will die quicker, and can't kill as many high lvl hostiles.</t>
+  </si>
+  <si>
+    <t>Borg Level 29 Hostiles</t>
+  </si>
+  <si>
+    <t>Eclipse Hostiles</t>
+  </si>
+  <si>
+    <t>"Moreau", "Pike", "Chen"</t>
+  </si>
+  <si>
+    <t>A crew for level 29 Borg hostiles</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>"Marcus", "Yuki", "Harrison"</t>
+  </si>
+  <si>
+    <t>D4 Anti-Explorer Primary</t>
+  </si>
+  <si>
+    <t>"Marcus", "Yuki", "Khan"</t>
+  </si>
+  <si>
+    <t>D4 Anti-Explorer Secondary</t>
+  </si>
+  <si>
+    <t>A very good crew versus Explorers, especially enterprises</t>
+  </si>
+  <si>
+    <t>The most basic crew versus explorers, If you have Harrison or Worf replace Khan with one of them, Not tried enough to know which</t>
+  </si>
+  <si>
+    <t>D4 Anti-Explorer Tertiary</t>
+  </si>
+  <si>
+    <t>"Marcus","Yuki","Honorguard Worf"</t>
+  </si>
+  <si>
+    <t>A very good crew versus Explorers.</t>
+  </si>
+  <si>
+    <t>Stella Primary Hostile</t>
+  </si>
+  <si>
+    <t>Default crew for hitting Eclipses</t>
+  </si>
+  <si>
+    <t>Swarms Tertiary</t>
+  </si>
+  <si>
+    <t>"Moreau", "Pike", "Jaylah (not Borg)"</t>
   </si>
 </sst>
 </file>
@@ -644,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79ED9618-281F-4DFD-8A89-B84C2E745081}">
   <dimension ref="A1:M614"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,19 +802,19 @@
     </row>
     <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -772,19 +823,19 @@
     </row>
     <row r="6" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -793,19 +844,19 @@
     </row>
     <row r="7" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>41</v>
@@ -813,140 +864,140 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -954,64 +1005,148 @@
         <v>60</v>
       </c>
       <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>